<commit_message>
Take handle as input from user
</commit_message>
<xml_diff>
--- a/features.xlsx
+++ b/features.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
+    <sheet name="Tasks" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>TODO</t>
   </si>
@@ -45,19 +46,34 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Features</t>
-  </si>
-  <si>
-    <t>CFS_1</t>
-  </si>
-  <si>
-    <t>CFS_2</t>
-  </si>
-  <si>
-    <t>CFS_3</t>
-  </si>
-  <si>
-    <t>CFS_4</t>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>F_1</t>
+  </si>
+  <si>
+    <t>F_2</t>
+  </si>
+  <si>
+    <t>F_3</t>
+  </si>
+  <si>
+    <t>F_4</t>
+  </si>
+  <si>
+    <t>T_1</t>
+  </si>
+  <si>
+    <t>Take handle as input from the user</t>
+  </si>
+  <si>
+    <t>T_2</t>
+  </si>
+  <si>
+    <t>Call a basic api and print json data to console</t>
   </si>
 </sst>
 </file>
@@ -105,7 +121,40 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="14">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -130,18 +179,6 @@
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -156,14 +193,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E5" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E5" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:E5"/>
   <tableColumns count="5">
+    <tableColumn id="1" name="ID" dataDxfId="11"/>
+    <tableColumn id="2" name="Feature" dataDxfId="10"/>
+    <tableColumn id="5" name="TODO" dataDxfId="7"/>
+    <tableColumn id="6" name="In Progress" dataDxfId="9"/>
+    <tableColumn id="4" name="Done" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:E3" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:E3"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="ID" dataDxfId="6"/>
-    <tableColumn id="2" name="Features" dataDxfId="5"/>
-    <tableColumn id="5" name="TODO" dataDxfId="0"/>
-    <tableColumn id="6" name="In Progress" dataDxfId="1"/>
-    <tableColumn id="4" name="Done" dataDxfId="4"/>
+    <tableColumn id="2" name="Task" dataDxfId="5"/>
+    <tableColumn id="3" name="TODO" dataDxfId="4"/>
+    <tableColumn id="4" name="In Progress" dataDxfId="3"/>
+    <tableColumn id="5" name="Done" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -434,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +504,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -467,46 +518,46 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -516,4 +567,69 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="57.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>